<commit_message>
create excel file with colour coded mapping
</commit_message>
<xml_diff>
--- a/RawData/IDs_mapping_color.xlsx
+++ b/RawData/IDs_mapping_color.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Dropbox/Home/College/Edinburgh - MSc Data Science/Big Data Analytics/diabetes_readmissions/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08802648-E91D-9742-8ACF-548A463F5A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{734C5E9D-6A3B-D64B-84FD-AB7D621E8CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,7 +1266,7 @@
       <c r="A21">
         <v>10</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
       <c r="A23">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created graph scripts medical speciality
</commit_message>
<xml_diff>
--- a/RawData/IDs_mapping_color.xlsx
+++ b/RawData/IDs_mapping_color.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11106"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/Dropbox/Home/College/Edinburgh - MSc Data Science/Big Data Analytics/diabetes_readmissions/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{734C5E9D-6A3B-D64B-84FD-AB7D621E8CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517C9FB5-95D6-C847-919A-326D4A5EFFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IDs_mapping" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1101,11 +1101,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>